<commit_message>
Prelim work on localization
</commit_message>
<xml_diff>
--- a/Sets-SATIMGE.xlsx
+++ b/Sets-SATIMGE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C627FE17-D0FD-4A69-ACDB-15829442866D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750B8E3C-3924-461B-BFC2-2E00211F07C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1215" windowWidth="26610" windowHeight="13740" activeTab="1" xr2:uid="{008F860A-1793-4F78-8899-BE3F7B7A437A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{008F860A-1793-4F78-8899-BE3F7B7A437A}"/>
   </bookViews>
   <sheets>
     <sheet name="SetsEditor- Proc" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="117">
   <si>
     <t>~TFM_Psets</t>
   </si>
@@ -263,6 +263,132 @@
   </si>
   <si>
     <t>TP*,-TPR*</t>
+  </si>
+  <si>
+    <t>EPumpStorage</t>
+  </si>
+  <si>
+    <t>EBiomass</t>
+  </si>
+  <si>
+    <t>EHydro</t>
+  </si>
+  <si>
+    <t>EImports</t>
+  </si>
+  <si>
+    <t>EPV_Grid</t>
+  </si>
+  <si>
+    <t>EPV_RfTpIND</t>
+  </si>
+  <si>
+    <t>ECSP</t>
+  </si>
+  <si>
+    <t>EWind</t>
+  </si>
+  <si>
+    <t>EBattery-Commerce</t>
+  </si>
+  <si>
+    <t>EBattery-Utility</t>
+  </si>
+  <si>
+    <t>EGas</t>
+  </si>
+  <si>
+    <t>ENuclear</t>
+  </si>
+  <si>
+    <t>EOil</t>
+  </si>
+  <si>
+    <t>Etrans</t>
+  </si>
+  <si>
+    <t>Edist_Residential</t>
+  </si>
+  <si>
+    <t>Edist_Agriculture</t>
+  </si>
+  <si>
+    <t>Edist_Industry</t>
+  </si>
+  <si>
+    <t>Edist_Commercial</t>
+  </si>
+  <si>
+    <t>Edist_Transport</t>
+  </si>
+  <si>
+    <t>EPTSTO*</t>
+  </si>
+  <si>
+    <t>ERB*</t>
+  </si>
+  <si>
+    <t>ERHYD*,-ERHYD*-I</t>
+  </si>
+  <si>
+    <t>ERHYD*-I</t>
+  </si>
+  <si>
+    <t>ERSOLPC*</t>
+  </si>
+  <si>
+    <t>ERSOLT*</t>
+  </si>
+  <si>
+    <t>ERWND*</t>
+  </si>
+  <si>
+    <t>ESTSU*</t>
+  </si>
+  <si>
+    <t>ECoal</t>
+  </si>
+  <si>
+    <t>ETC*</t>
+  </si>
+  <si>
+    <t>ETG*</t>
+  </si>
+  <si>
+    <t>ETN*</t>
+  </si>
+  <si>
+    <t>ETO*</t>
+  </si>
+  <si>
+    <t>ETRANS*</t>
+  </si>
+  <si>
+    <t>XRESELC</t>
+  </si>
+  <si>
+    <t>XAGRELC</t>
+  </si>
+  <si>
+    <t>XCOMELC</t>
+  </si>
+  <si>
+    <t>XI*ELC,XU*ELC</t>
+  </si>
+  <si>
+    <t>XTRAELC</t>
+  </si>
+  <si>
+    <t>EPV_RfT</t>
+  </si>
+  <si>
+    <t>ESTSC*,ESTSI*,ESTSR*</t>
+  </si>
+  <si>
+    <t>EBattery-Dist</t>
+  </si>
+  <si>
+    <t>ERSOLPI*,ERSOLPRC*,ERSOLPRR*</t>
   </si>
 </sst>
 </file>
@@ -614,10 +740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{263D98BE-72FA-4B80-B173-2E4676308DDA}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,7 +752,7 @@
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1"/>
     <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="8.140625" bestFit="1" customWidth="1"/>
@@ -853,6 +979,226 @@
         <v>74</v>
       </c>
     </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>75</v>
+      </c>
+      <c r="F12" t="s">
+        <v>75</v>
+      </c>
+      <c r="H12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F13" t="s">
+        <v>76</v>
+      </c>
+      <c r="H13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F14" t="s">
+        <v>77</v>
+      </c>
+      <c r="H14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>78</v>
+      </c>
+      <c r="F15" t="s">
+        <v>78</v>
+      </c>
+      <c r="H15" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16" t="s">
+        <v>79</v>
+      </c>
+      <c r="H16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>113</v>
+      </c>
+      <c r="F17" t="s">
+        <v>80</v>
+      </c>
+      <c r="H17" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" t="s">
+        <v>81</v>
+      </c>
+      <c r="H18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>82</v>
+      </c>
+      <c r="F19" t="s">
+        <v>82</v>
+      </c>
+      <c r="H19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>115</v>
+      </c>
+      <c r="F20" t="s">
+        <v>83</v>
+      </c>
+      <c r="H20" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>84</v>
+      </c>
+      <c r="F21" t="s">
+        <v>84</v>
+      </c>
+      <c r="H21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>102</v>
+      </c>
+      <c r="F22" t="s">
+        <v>102</v>
+      </c>
+      <c r="H22" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>85</v>
+      </c>
+      <c r="F23" t="s">
+        <v>85</v>
+      </c>
+      <c r="H23" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>86</v>
+      </c>
+      <c r="F24" t="s">
+        <v>86</v>
+      </c>
+      <c r="H24" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>87</v>
+      </c>
+      <c r="F25" t="s">
+        <v>87</v>
+      </c>
+      <c r="H25" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>88</v>
+      </c>
+      <c r="F26" t="s">
+        <v>88</v>
+      </c>
+      <c r="H26" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="27" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>89</v>
+      </c>
+      <c r="F27" t="s">
+        <v>89</v>
+      </c>
+      <c r="H27" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>90</v>
+      </c>
+      <c r="F28" t="s">
+        <v>90</v>
+      </c>
+      <c r="H28" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="29" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>91</v>
+      </c>
+      <c r="F29" t="s">
+        <v>91</v>
+      </c>
+      <c r="H29" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="30" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>92</v>
+      </c>
+      <c r="F30" t="s">
+        <v>92</v>
+      </c>
+      <c r="H30" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>93</v>
+      </c>
+      <c r="F31" t="s">
+        <v>93</v>
+      </c>
+      <c r="H31" t="s">
+        <v>112</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -862,7 +1208,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BD03DB1-DD55-4548-B86E-1F92E13CF8ED}">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1063,7 +1409,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:J1048576"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
TIMES files finalised for localization work
</commit_message>
<xml_diff>
--- a/Sets-SATIMGE.xlsx
+++ b/Sets-SATIMGE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750B8E3C-3924-461B-BFC2-2E00211F07C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A5CB828-7AB7-45BF-BC74-9ADC9C6950DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{008F860A-1793-4F78-8899-BE3F7B7A437A}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="115">
   <si>
     <t>~TFM_Psets</t>
   </si>
@@ -280,21 +280,12 @@
     <t>EPV_Grid</t>
   </si>
   <si>
-    <t>EPV_RfTpIND</t>
-  </si>
-  <si>
     <t>ECSP</t>
   </si>
   <si>
     <t>EWind</t>
   </si>
   <si>
-    <t>EBattery-Commerce</t>
-  </si>
-  <si>
-    <t>EBattery-Utility</t>
-  </si>
-  <si>
     <t>EGas</t>
   </si>
   <si>
@@ -379,16 +370,19 @@
     <t>XTRAELC</t>
   </si>
   <si>
-    <t>EPV_RfT</t>
-  </si>
-  <si>
     <t>ESTSC*,ESTSI*,ESTSR*</t>
   </si>
   <si>
-    <t>EBattery-Dist</t>
-  </si>
-  <si>
-    <t>ERSOLPI*,ERSOLPRC*,ERSOLPRR*</t>
+    <t>EPV_RfTp</t>
+  </si>
+  <si>
+    <t>ERSOLPRI*,ERSOLPRC*,ERSOLPRR*</t>
+  </si>
+  <si>
+    <t>Ebattery_Dist</t>
+  </si>
+  <si>
+    <t>Ebattery_Utility</t>
   </si>
 </sst>
 </file>
@@ -743,7 +737,7 @@
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD19"/>
+      <selection activeCell="F20" sqref="F20:F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,7 +981,7 @@
         <v>75</v>
       </c>
       <c r="H12" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -998,7 +992,7 @@
         <v>76</v>
       </c>
       <c r="H13" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1009,7 +1003,7 @@
         <v>77</v>
       </c>
       <c r="H14" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1020,7 +1014,7 @@
         <v>78</v>
       </c>
       <c r="H15" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1031,172 +1025,172 @@
         <v>79</v>
       </c>
       <c r="H16" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F17" t="s">
-        <v>80</v>
+        <v>111</v>
       </c>
       <c r="H17" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H18" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H19" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F20" t="s">
-        <v>83</v>
+        <v>113</v>
       </c>
       <c r="H20" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
-        <v>84</v>
+        <v>114</v>
       </c>
       <c r="F21" t="s">
-        <v>84</v>
+        <v>114</v>
       </c>
       <c r="H21" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E22" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F22" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H22" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F23" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H23" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F24" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H24" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E25" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F25" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H25" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F26" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H26" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E27" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F27" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H27" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E28" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F28" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H28" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F29" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H29" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E30" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F30" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H30" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E31" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F31" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="H31" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Testing Sankeys with Loops
</commit_message>
<xml_diff>
--- a/Sets-SATIMGE.xlsx
+++ b/Sets-SATIMGE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F7C765-2AFA-4C82-980C-A23B7D37E993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{106B0B48-80E0-4B47-86BE-8451FA379F0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3675" yWindow="-19785" windowWidth="36795" windowHeight="18975" activeTab="1" xr2:uid="{008F860A-1793-4F78-8899-BE3F7B7A437A}"/>
+    <workbookView xWindow="4170" yWindow="-21195" windowWidth="36795" windowHeight="18975" xr2:uid="{008F860A-1793-4F78-8899-BE3F7B7A437A}"/>
   </bookViews>
   <sheets>
     <sheet name="SetsEditor- Proc" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1173" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1179" uniqueCount="546">
   <si>
     <t>SetName</t>
   </si>
@@ -1681,7 +1681,13 @@
     <t>AT*,I??R*,-IPPREC*</t>
   </si>
   <si>
-    <t>FinalEnergy-Exports</t>
+    <t>FinalEnergy</t>
+  </si>
+  <si>
+    <t>IND_ElecGenDist</t>
+  </si>
+  <si>
+    <t>I??ELC</t>
   </si>
 </sst>
 </file>
@@ -2063,13 +2069,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{263D98BE-72FA-4B80-B173-2E4676308DDA}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:N141"/>
+  <dimension ref="A1:N142"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="E45" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H82" sqref="H82"/>
+      <selection pane="bottomRight" activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2502,13 +2508,16 @@
     </row>
     <row r="24" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E24" t="s">
-        <v>121</v>
+        <v>544</v>
       </c>
       <c r="F24" t="s">
-        <v>121</v>
+        <v>544</v>
       </c>
       <c r="H24" t="s">
-        <v>125</v>
+        <v>133</v>
+      </c>
+      <c r="J24" t="s">
+        <v>545</v>
       </c>
       <c r="M24" t="s">
         <v>120</v>
@@ -2519,13 +2528,13 @@
     </row>
     <row r="25" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E25" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F25" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H25" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="M25" t="s">
         <v>120</v>
@@ -2536,13 +2545,13 @@
     </row>
     <row r="26" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H26" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="M26" t="s">
         <v>120</v>
@@ -2553,13 +2562,13 @@
     </row>
     <row r="27" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E27" t="s">
-        <v>218</v>
+        <v>123</v>
       </c>
       <c r="F27" t="s">
-        <v>218</v>
+        <v>123</v>
       </c>
       <c r="H27" t="s">
-        <v>219</v>
+        <v>126</v>
       </c>
       <c r="M27" t="s">
         <v>120</v>
@@ -2570,13 +2579,13 @@
     </row>
     <row r="28" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E28" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="F28" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="H28" t="s">
-        <v>235</v>
+        <v>219</v>
       </c>
       <c r="M28" t="s">
         <v>120</v>
@@ -2587,13 +2596,13 @@
     </row>
     <row r="29" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E29" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F29" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="H29" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="M29" t="s">
         <v>120</v>
@@ -2604,13 +2613,13 @@
     </row>
     <row r="30" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E30" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="F30" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="H30" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="M30" t="s">
         <v>120</v>
@@ -2621,13 +2630,13 @@
     </row>
     <row r="31" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E31" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="F31" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="H31" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="M31" t="s">
         <v>120</v>
@@ -2638,13 +2647,13 @@
     </row>
     <row r="32" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E32" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F32" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H32" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="M32" t="s">
         <v>120</v>
@@ -2655,13 +2664,13 @@
     </row>
     <row r="33" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E33" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F33" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="H33" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="M33" t="s">
         <v>120</v>
@@ -2672,13 +2681,13 @@
     </row>
     <row r="34" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E34" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F34" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H34" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="M34" t="s">
         <v>120</v>
@@ -2689,13 +2698,13 @@
     </row>
     <row r="35" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E35" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F35" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H35" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="M35" t="s">
         <v>120</v>
@@ -2706,13 +2715,13 @@
     </row>
     <row r="36" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E36" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F36" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H36" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="M36" t="s">
         <v>120</v>
@@ -2723,13 +2732,13 @@
     </row>
     <row r="37" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E37" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F37" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H37" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="M37" t="s">
         <v>120</v>
@@ -2740,13 +2749,13 @@
     </row>
     <row r="38" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E38" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F38" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H38" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="M38" t="s">
         <v>120</v>
@@ -2757,13 +2766,13 @@
     </row>
     <row r="39" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E39" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F39" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H39" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="M39" t="s">
         <v>120</v>
@@ -2774,13 +2783,13 @@
     </row>
     <row r="40" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E40" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F40" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H40" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="M40" t="s">
         <v>120</v>
@@ -2791,13 +2800,13 @@
     </row>
     <row r="41" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E41" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F41" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H41" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="M41" t="s">
         <v>120</v>
@@ -2808,13 +2817,13 @@
     </row>
     <row r="42" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E42" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F42" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H42" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="M42" t="s">
         <v>120</v>
@@ -2825,13 +2834,13 @@
     </row>
     <row r="43" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E43" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F43" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H43" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="M43" t="s">
         <v>120</v>
@@ -2842,13 +2851,13 @@
     </row>
     <row r="44" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E44" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F44" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H44" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="M44" t="s">
         <v>120</v>
@@ -2859,13 +2868,13 @@
     </row>
     <row r="45" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E45" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F45" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H45" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="M45" t="s">
         <v>120</v>
@@ -2876,13 +2885,13 @@
     </row>
     <row r="46" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E46" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F46" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H46" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="M46" t="s">
         <v>120</v>
@@ -2893,13 +2902,13 @@
     </row>
     <row r="47" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E47" t="s">
-        <v>298</v>
+        <v>265</v>
       </c>
       <c r="F47" t="s">
-        <v>299</v>
+        <v>265</v>
       </c>
       <c r="H47" t="s">
-        <v>300</v>
+        <v>279</v>
       </c>
       <c r="M47" t="s">
         <v>120</v>
@@ -2910,13 +2919,13 @@
     </row>
     <row r="48" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E48" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="F48" t="s">
-        <v>309</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>310</v>
+        <v>299</v>
+      </c>
+      <c r="H48" t="s">
+        <v>300</v>
       </c>
       <c r="M48" t="s">
         <v>120</v>
@@ -2927,13 +2936,13 @@
     </row>
     <row r="49" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E49" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="F49" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
       <c r="M49" t="s">
         <v>120</v>
@@ -2944,13 +2953,13 @@
     </row>
     <row r="50" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E50" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F50" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="M50" t="s">
         <v>120</v>
@@ -2961,13 +2970,13 @@
     </row>
     <row r="51" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E51" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F51" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="M51" t="s">
         <v>120</v>
@@ -2978,13 +2987,13 @@
     </row>
     <row r="52" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E52" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F52" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="M52" t="s">
         <v>120</v>
@@ -2995,13 +3004,13 @@
     </row>
     <row r="53" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E53" t="s">
-        <v>24</v>
+        <v>320</v>
       </c>
       <c r="F53" t="s">
-        <v>24</v>
-      </c>
-      <c r="H53" t="s">
-        <v>34</v>
+        <v>320</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>324</v>
       </c>
       <c r="M53" t="s">
         <v>120</v>
@@ -3012,13 +3021,13 @@
     </row>
     <row r="54" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E54" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F54" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H54" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M54" t="s">
         <v>120</v>
@@ -3029,13 +3038,13 @@
     </row>
     <row r="55" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E55" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F55" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H55" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M55" t="s">
         <v>120</v>
@@ -3046,13 +3055,13 @@
     </row>
     <row r="56" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E56" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F56" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H56" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M56" t="s">
         <v>120</v>
@@ -3063,13 +3072,13 @@
     </row>
     <row r="57" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E57" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F57" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H57" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M57" t="s">
         <v>120</v>
@@ -3080,13 +3089,13 @@
     </row>
     <row r="58" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E58" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="F58" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="H58" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="M58" t="s">
         <v>120</v>
@@ -3097,13 +3106,13 @@
     </row>
     <row r="59" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E59" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="F59" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="H59" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="M59" t="s">
         <v>120</v>
@@ -3114,13 +3123,13 @@
     </row>
     <row r="60" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E60" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F60" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H60" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M60" t="s">
         <v>120</v>
@@ -3131,13 +3140,13 @@
     </row>
     <row r="61" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E61" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="F61" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="H61" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="M61" t="s">
         <v>120</v>
@@ -3148,13 +3157,13 @@
     </row>
     <row r="62" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E62" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F62" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H62" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="M62" t="s">
         <v>120</v>
@@ -3165,13 +3174,13 @@
     </row>
     <row r="63" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E63" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="F63" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="H63" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="M63" t="s">
         <v>120</v>
@@ -3182,13 +3191,13 @@
     </row>
     <row r="64" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E64" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="F64" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="H64" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M64" t="s">
         <v>120</v>
@@ -3199,13 +3208,13 @@
     </row>
     <row r="65" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E65" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F65" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H65" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M65" t="s">
         <v>120</v>
@@ -3216,13 +3225,13 @@
     </row>
     <row r="66" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E66" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F66" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H66" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M66" t="s">
         <v>120</v>
@@ -3233,32 +3242,31 @@
     </row>
     <row r="67" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E67" t="s">
-        <v>535</v>
+        <v>33</v>
       </c>
       <c r="F67" t="s">
-        <v>535</v>
-      </c>
-      <c r="H67" t="str">
-        <f>H70&amp;","&amp;H74&amp;","&amp;H75&amp;","&amp;H76&amp;","&amp;H77&amp;","&amp;H80</f>
-        <v>R??K*,C?K*,R??R*,C?R*,R??H*,C?H*,R??W*,C?W*,C?C*,I??C*,-IPPCHE*,-INMC*,-IMP*,-IIS*,I??H*,AH*,I??S*,I??K*,IALPOT,I??EAF*,IPPSTM*,IALPOTINERT,ICPSGAS-E,INMBRISTD,INMCEMK*,INMGLASTD,INMLIMSTD,IPG*,IIS*,IFCEAF*,IFMEAF*,-IISCOV*,-IISHALKHGN,-IISHGN*,-IISHDRI*,-IISMOE*,-IISSALDHGN,-IMISHGN*,-IOTSHGN*,-IFBSHGN*,-ICPSHGN*,-IPPSTMBLQ*</v>
+        <v>33</v>
+      </c>
+      <c r="H67" t="s">
+        <v>46</v>
       </c>
       <c r="M67" t="s">
-        <v>72</v>
+        <v>120</v>
       </c>
       <c r="N67" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
     </row>
     <row r="68" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E68" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="F68" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="H68" t="str">
-        <f>H79&amp;","&amp;H81&amp;","&amp;H82&amp;","&amp;H7</f>
-        <v>C?T*,AI*,AP*I??A*,I??P*,I??F*,-IALPOT,-IALPOTINERT,-IISPELTS-N,IPPPAP*,I??O*,INMCEMP*,INMCEMFGRP,INMCEMFGBM,AT*,I??R*,-IPPREC*,T*</v>
+        <f>H71&amp;","&amp;H75&amp;","&amp;H76&amp;","&amp;H77&amp;","&amp;H78&amp;","&amp;H81</f>
+        <v>R??K*,C?K*,R??R*,C?R*,R??H*,C?H*,R??W*,C?W*,C?C*,I??C*,-IPPCHE*,-INMC*,-IMP*,-IIS*,I??H*,AH*,I??S*,I??K*,IALPOT,I??EAF*,IPPSTM*,IALPOTINERT,ICPSGAS-E,INMBRISTD,INMCEMK*,INMGLASTD,INMLIMSTD,IPG*,IIS*,IFCEAF*,IFMEAF*,-IISCOV*,-IISHALKHGN,-IISHGN*,-IISHDRI*,-IISMOE*,-IISSALDHGN,-IMISHGN*,-IOTSHGN*,-IFBSHGN*,-ICPSHGN*,-IPPSTMBLQ*</v>
       </c>
       <c r="M68" t="s">
         <v>72</v>
@@ -3269,14 +3277,14 @@
     </row>
     <row r="69" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E69" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F69" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="H69" t="str">
-        <f>H71&amp;","&amp;H72&amp;","&amp;H73&amp;","&amp;H78&amp;","&amp;H82</f>
-        <v>R??L*,C?L*,I??L*,-INM*,,R??N*,ICPGASNH3-E,ICPTGMU*,C?N*,AO*,R??O*,C?O*,I??E*,-IPPSTM*,-IMP*,-IIS*,-IFM*,-IFC*,INMCLI*,IPP*,-IPGM*,-IPPPAP*,-IPPSTM*,-IPPELC*,C?G*,AT*,I??R*,-IPPREC*</v>
+        <f>H80&amp;","&amp;H82&amp;","&amp;H83&amp;","&amp;H7</f>
+        <v>C?T*,AI*,AP*I??A*,I??P*,I??F*,-IALPOT,-IALPOTINERT,-IISPELTS-N,IPPPAP*,I??O*,INMCEMP*,INMCEMFGRP,INMCEMFGBM,AT*,I??R*,-IPPREC*,T*</v>
       </c>
       <c r="M69" t="s">
         <v>72</v>
@@ -3287,16 +3295,17 @@
     </row>
     <row r="70" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E70" t="s">
-        <v>113</v>
+        <v>537</v>
       </c>
       <c r="F70" t="s">
-        <v>113</v>
-      </c>
-      <c r="H70" t="s">
-        <v>240</v>
+        <v>537</v>
+      </c>
+      <c r="H70" t="str">
+        <f>H72&amp;","&amp;H73&amp;","&amp;H74&amp;","&amp;H79&amp;","&amp;H83</f>
+        <v>R??L*,C?L*,I??L*,-INM*,,R??N*,ICPGASNH3-E,ICPTGMU*,C?N*,AO*,R??O*,C?O*,I??E*,-IPPSTM*,-IMP*,-IIS*,-IFM*,-IFC*,INMCLI*,IPP*,-IPGM*,-IPPPAP*,-IPPSTM*,-IPPELC*,C?G*,AT*,I??R*,-IPPREC*</v>
       </c>
       <c r="M70" t="s">
-        <v>120</v>
+        <v>72</v>
       </c>
       <c r="N70" t="s">
         <v>114</v>
@@ -3304,13 +3313,13 @@
     </row>
     <row r="71" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E71" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F71" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H71" t="s">
-        <v>288</v>
+        <v>240</v>
       </c>
       <c r="M71" t="s">
         <v>120</v>
@@ -3320,15 +3329,14 @@
       </c>
     </row>
     <row r="72" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="E72" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="F72" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="G72" s="2"/>
-      <c r="H72" s="2" t="s">
-        <v>362</v>
+      <c r="E72" t="s">
+        <v>115</v>
+      </c>
+      <c r="F72" t="s">
+        <v>115</v>
+      </c>
+      <c r="H72" t="s">
+        <v>288</v>
       </c>
       <c r="M72" t="s">
         <v>120</v>
@@ -3339,14 +3347,14 @@
     </row>
     <row r="73" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E73" s="2" t="s">
-        <v>116</v>
+        <v>281</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>116</v>
+        <v>281</v>
       </c>
       <c r="G73" s="2"/>
       <c r="H73" s="2" t="s">
-        <v>539</v>
+        <v>362</v>
       </c>
       <c r="M73" t="s">
         <v>120</v>
@@ -3357,14 +3365,14 @@
     </row>
     <row r="74" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E74" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G74" s="2"/>
       <c r="H74" s="2" t="s">
-        <v>241</v>
+        <v>539</v>
       </c>
       <c r="M74" t="s">
         <v>120</v>
@@ -3375,14 +3383,14 @@
     </row>
     <row r="75" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E75" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G75" s="2"/>
       <c r="H75" s="2" t="s">
-        <v>292</v>
+        <v>241</v>
       </c>
       <c r="M75" t="s">
         <v>120</v>
@@ -3393,14 +3401,14 @@
     </row>
     <row r="76" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E76" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G76" s="2"/>
       <c r="H76" s="2" t="s">
-        <v>242</v>
+        <v>292</v>
       </c>
       <c r="M76" t="s">
         <v>120</v>
@@ -3411,14 +3419,14 @@
     </row>
     <row r="77" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E77" s="2" t="s">
-        <v>243</v>
+        <v>119</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>243</v>
+        <v>119</v>
       </c>
       <c r="G77" s="2"/>
       <c r="H77" s="2" t="s">
-        <v>293</v>
+        <v>242</v>
       </c>
       <c r="M77" t="s">
         <v>120</v>
@@ -3427,21 +3435,17 @@
         <v>114</v>
       </c>
     </row>
-    <row r="78" spans="5:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E78" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G78" s="2"/>
       <c r="H78" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="I78"/>
-      <c r="J78"/>
-      <c r="K78"/>
-      <c r="L78"/>
+        <v>293</v>
+      </c>
       <c r="M78" t="s">
         <v>120</v>
       </c>
@@ -3449,17 +3453,21 @@
         <v>114</v>
       </c>
     </row>
-    <row r="79" spans="5:14" x14ac:dyDescent="0.35">
+    <row r="79" spans="5:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="E79" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G79" s="2"/>
       <c r="H79" s="2" t="s">
-        <v>247</v>
-      </c>
+        <v>246</v>
+      </c>
+      <c r="I79"/>
+      <c r="J79"/>
+      <c r="K79"/>
+      <c r="L79"/>
       <c r="M79" t="s">
         <v>120</v>
       </c>
@@ -3469,14 +3477,14 @@
     </row>
     <row r="80" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E80" s="2" t="s">
-        <v>280</v>
+        <v>245</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>280</v>
+        <v>245</v>
       </c>
       <c r="G80" s="2"/>
       <c r="H80" s="2" t="s">
-        <v>538</v>
+        <v>247</v>
       </c>
       <c r="M80" t="s">
         <v>120</v>
@@ -3487,32 +3495,32 @@
     </row>
     <row r="81" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E81" s="2" t="s">
-        <v>330</v>
+        <v>280</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>330</v>
+        <v>280</v>
       </c>
       <c r="G81" s="2"/>
       <c r="H81" s="2" t="s">
-        <v>540</v>
-      </c>
-      <c r="M81" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="N81" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="M81" t="s">
+        <v>120</v>
+      </c>
+      <c r="N81" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="82" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E82" s="2" t="s">
-        <v>541</v>
+        <v>330</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>541</v>
+        <v>330</v>
       </c>
       <c r="G82" s="2"/>
       <c r="H82" s="2" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="M82" s="2" t="s">
         <v>120</v>
@@ -3523,13 +3531,14 @@
     </row>
     <row r="83" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E83" s="2" t="s">
-        <v>325</v>
+        <v>541</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>325</v>
-      </c>
+        <v>541</v>
+      </c>
+      <c r="G83" s="2"/>
       <c r="H83" s="2" t="s">
-        <v>424</v>
+        <v>542</v>
       </c>
       <c r="M83" s="2" t="s">
         <v>120</v>
@@ -3540,13 +3549,13 @@
     </row>
     <row r="84" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E84" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H84" s="2" t="s">
-        <v>327</v>
+        <v>424</v>
       </c>
       <c r="M84" s="2" t="s">
         <v>120</v>
@@ -3557,13 +3566,13 @@
     </row>
     <row r="85" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E85" s="2" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="H85" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="M85" s="2" t="s">
         <v>120</v>
@@ -3572,32 +3581,32 @@
         <v>114</v>
       </c>
     </row>
-    <row r="86" spans="5:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E86" s="2" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>348</v>
+        <v>328</v>
       </c>
       <c r="M86" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="N86" t="s">
-        <v>124</v>
+      <c r="N86" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="87" spans="5:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="E87" s="2" t="s">
-        <v>365</v>
+        <v>332</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>365</v>
+        <v>332</v>
       </c>
       <c r="H87" s="2" t="s">
-        <v>395</v>
+        <v>348</v>
       </c>
       <c r="M87" s="2" t="s">
         <v>120</v>
@@ -3608,13 +3617,13 @@
     </row>
     <row r="88" spans="5:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="E88" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="H88" s="2" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="M88" s="2" t="s">
         <v>120</v>
@@ -3625,13 +3634,13 @@
     </row>
     <row r="89" spans="5:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="E89" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>396</v>
+        <v>367</v>
       </c>
       <c r="H89" s="2" t="s">
-        <v>383</v>
+        <v>394</v>
       </c>
       <c r="M89" s="2" t="s">
         <v>120</v>
@@ -3642,13 +3651,13 @@
     </row>
     <row r="90" spans="5:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="E90" s="2" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>366</v>
+        <v>396</v>
       </c>
       <c r="H90" s="2" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="M90" s="2" t="s">
         <v>120</v>
@@ -3659,13 +3668,13 @@
     </row>
     <row r="91" spans="5:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="E91" s="2" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="H91" s="2" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="M91" s="2" t="s">
         <v>120</v>
@@ -3676,13 +3685,13 @@
     </row>
     <row r="92" spans="5:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="E92" s="2" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="H92" s="2" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="M92" s="2" t="s">
         <v>120</v>
@@ -3693,13 +3702,13 @@
     </row>
     <row r="93" spans="5:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="E93" s="2" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="H93" s="2" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="M93" s="2" t="s">
         <v>120</v>
@@ -3710,13 +3719,13 @@
     </row>
     <row r="94" spans="5:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="E94" s="2" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="M94" s="2" t="s">
         <v>120</v>
@@ -3727,13 +3736,13 @@
     </row>
     <row r="95" spans="5:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="E95" s="2" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>397</v>
+        <v>369</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="M95" s="2" t="s">
         <v>120</v>
@@ -3744,13 +3753,13 @@
     </row>
     <row r="96" spans="5:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="E96" s="2" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>371</v>
+        <v>397</v>
       </c>
       <c r="H96" s="2" t="s">
-        <v>351</v>
+        <v>377</v>
       </c>
       <c r="M96" s="2" t="s">
         <v>120</v>
@@ -3761,13 +3770,13 @@
     </row>
     <row r="97" spans="5:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="E97" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="H97" s="2" t="s">
-        <v>376</v>
+        <v>351</v>
       </c>
       <c r="M97" s="2" t="s">
         <v>120</v>
@@ -3778,13 +3787,13 @@
     </row>
     <row r="98" spans="5:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="E98" s="2" t="s">
-        <v>333</v>
+        <v>373</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>333</v>
+        <v>373</v>
       </c>
       <c r="H98" s="2" t="s">
-        <v>393</v>
+        <v>376</v>
       </c>
       <c r="M98" s="2" t="s">
         <v>120</v>
@@ -3795,13 +3804,13 @@
     </row>
     <row r="99" spans="5:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="E99" s="2" t="s">
-        <v>374</v>
+        <v>333</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>374</v>
+        <v>333</v>
       </c>
       <c r="H99" s="2" t="s">
-        <v>349</v>
+        <v>393</v>
       </c>
       <c r="M99" s="2" t="s">
         <v>120</v>
@@ -3812,30 +3821,30 @@
     </row>
     <row r="100" spans="5:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="E100" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="H100" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="M100" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="N100" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="101" spans="5:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="E101" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="F100" s="2" t="s">
+      <c r="F101" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="H100" s="2" t="s">
+      <c r="H101" s="2" t="s">
         <v>350</v>
-      </c>
-      <c r="M100" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="N100" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="101" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="E101" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="F101" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="H101" s="2" t="s">
-        <v>337</v>
       </c>
       <c r="M101" s="2" t="s">
         <v>120</v>
@@ -3846,13 +3855,13 @@
     </row>
     <row r="102" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E102" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H102" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="M102" s="2" t="s">
         <v>120</v>
@@ -3863,13 +3872,13 @@
     </row>
     <row r="103" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E103" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H103" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="M103" s="2" t="s">
         <v>120</v>
@@ -3880,13 +3889,13 @@
     </row>
     <row r="104" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E104" s="2" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="H104" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="M104" s="2" t="s">
         <v>120</v>
@@ -3897,13 +3906,13 @@
     </row>
     <row r="105" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E105" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="H105" s="2" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="M105" s="2" t="s">
         <v>120</v>
@@ -3914,13 +3923,13 @@
     </row>
     <row r="106" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E106" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H106" s="2" t="s">
-        <v>414</v>
+        <v>345</v>
       </c>
       <c r="M106" s="2" t="s">
         <v>120</v>
@@ -3931,13 +3940,13 @@
     </row>
     <row r="107" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E107" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="H107" s="2" t="s">
-        <v>346</v>
+        <v>414</v>
       </c>
       <c r="M107" s="2" t="s">
         <v>120</v>
@@ -3948,13 +3957,13 @@
     </row>
     <row r="108" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E108" s="2" t="s">
-        <v>417</v>
+        <v>344</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>417</v>
+        <v>344</v>
       </c>
       <c r="H108" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M108" s="2" t="s">
         <v>120</v>
@@ -3965,13 +3974,13 @@
     </row>
     <row r="109" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E109" s="2" t="s">
-        <v>352</v>
+        <v>417</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="H109" t="s">
-        <v>353</v>
+        <v>417</v>
+      </c>
+      <c r="H109" s="2" t="s">
+        <v>347</v>
       </c>
       <c r="M109" s="2" t="s">
         <v>120</v>
@@ -3982,15 +3991,15 @@
     </row>
     <row r="110" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E110" s="2" t="s">
-        <v>420</v>
+        <v>352</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>420</v>
+        <v>352</v>
       </c>
       <c r="H110" t="s">
-        <v>423</v>
-      </c>
-      <c r="M110" t="s">
+        <v>353</v>
+      </c>
+      <c r="M110" s="2" t="s">
         <v>120</v>
       </c>
       <c r="N110" t="s">
@@ -3999,13 +4008,13 @@
     </row>
     <row r="111" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E111" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H111" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="M111" t="s">
         <v>120</v>
@@ -4016,13 +4025,13 @@
     </row>
     <row r="112" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E112" s="2" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="H112" t="s">
-        <v>450</v>
+        <v>422</v>
       </c>
       <c r="M112" t="s">
         <v>120</v>
@@ -4033,14 +4042,13 @@
     </row>
     <row r="113" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E113" s="2" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>432</v>
-      </c>
-      <c r="G113" s="2"/>
+        <v>428</v>
+      </c>
       <c r="H113" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="M113" t="s">
         <v>120</v>
@@ -4051,14 +4059,14 @@
     </row>
     <row r="114" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E114" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="G114" s="2"/>
       <c r="H114" t="s">
-        <v>435</v>
+        <v>447</v>
       </c>
       <c r="M114" t="s">
         <v>120</v>
@@ -4069,13 +4077,14 @@
     </row>
     <row r="115" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E115" s="2" t="s">
-        <v>429</v>
+        <v>434</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>429</v>
-      </c>
+        <v>434</v>
+      </c>
+      <c r="G115" s="2"/>
       <c r="H115" t="s">
-        <v>489</v>
+        <v>435</v>
       </c>
       <c r="M115" t="s">
         <v>120</v>
@@ -4086,13 +4095,13 @@
     </row>
     <row r="116" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E116" s="2" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H116" t="s">
-        <v>440</v>
+        <v>489</v>
       </c>
       <c r="M116" t="s">
         <v>120</v>
@@ -4103,13 +4112,13 @@
     </row>
     <row r="117" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E117" s="2" t="s">
-        <v>430</v>
+        <v>441</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>430</v>
+        <v>441</v>
       </c>
       <c r="H117" t="s">
-        <v>431</v>
+        <v>440</v>
       </c>
       <c r="M117" t="s">
         <v>120</v>
@@ -4120,13 +4129,13 @@
     </row>
     <row r="118" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E118" s="2" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="H118" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
       <c r="M118" t="s">
         <v>120</v>
@@ -4137,14 +4146,13 @@
     </row>
     <row r="119" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E119" s="2" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="G119" s="2"/>
+        <v>436</v>
+      </c>
       <c r="H119" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="M119" t="s">
         <v>120</v>
@@ -4155,13 +4163,14 @@
     </row>
     <row r="120" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E120" s="2" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>442</v>
-      </c>
+        <v>438</v>
+      </c>
+      <c r="G120" s="2"/>
       <c r="H120" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="M120" t="s">
         <v>120</v>
@@ -4172,14 +4181,13 @@
     </row>
     <row r="121" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E121" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>444</v>
-      </c>
-      <c r="G121" s="2"/>
+        <v>442</v>
+      </c>
       <c r="H121" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="M121" t="s">
         <v>120</v>
@@ -4190,13 +4198,14 @@
     </row>
     <row r="122" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E122" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>446</v>
-      </c>
+        <v>444</v>
+      </c>
+      <c r="G122" s="2"/>
       <c r="H122" t="s">
-        <v>433</v>
+        <v>445</v>
       </c>
       <c r="M122" t="s">
         <v>120</v>
@@ -4207,13 +4216,13 @@
     </row>
     <row r="123" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E123" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="H123" t="s">
-        <v>449</v>
+        <v>433</v>
       </c>
       <c r="M123" t="s">
         <v>120</v>
@@ -4224,13 +4233,13 @@
     </row>
     <row r="124" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E124" s="2" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="H124" t="s">
-        <v>490</v>
+        <v>449</v>
       </c>
       <c r="M124" t="s">
         <v>120</v>
@@ -4241,13 +4250,13 @@
     </row>
     <row r="125" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E125" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="H125" t="s">
-        <v>497</v>
+        <v>490</v>
       </c>
       <c r="M125" t="s">
         <v>120</v>
@@ -4258,13 +4267,13 @@
     </row>
     <row r="126" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E126" s="2" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="H126" t="s">
-        <v>491</v>
+        <v>497</v>
       </c>
       <c r="M126" t="s">
         <v>120</v>
@@ -4275,13 +4284,13 @@
     </row>
     <row r="127" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E127" s="2" t="s">
-        <v>473</v>
+        <v>454</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>473</v>
+        <v>454</v>
       </c>
       <c r="H127" t="s">
-        <v>465</v>
+        <v>491</v>
       </c>
       <c r="M127" t="s">
         <v>120</v>
@@ -4292,13 +4301,13 @@
     </row>
     <row r="128" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E128" s="2" t="s">
-        <v>468</v>
+        <v>473</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>468</v>
+        <v>473</v>
       </c>
       <c r="H128" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="M128" t="s">
         <v>120</v>
@@ -4309,13 +4318,13 @@
     </row>
     <row r="129" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E129" s="2" t="s">
-        <v>455</v>
+        <v>468</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>455</v>
+        <v>468</v>
       </c>
       <c r="H129" t="s">
-        <v>461</v>
+        <v>469</v>
       </c>
       <c r="M129" t="s">
         <v>120</v>
@@ -4326,13 +4335,13 @@
     </row>
     <row r="130" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E130" s="2" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="F130" s="2" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="H130" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="M130" t="s">
         <v>120</v>
@@ -4343,13 +4352,13 @@
     </row>
     <row r="131" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E131" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="H131" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="M131" t="s">
         <v>120</v>
@@ -4360,13 +4369,13 @@
     </row>
     <row r="132" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E132" s="2" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="H132" t="s">
-        <v>459</v>
+        <v>467</v>
       </c>
       <c r="M132" t="s">
         <v>120</v>
@@ -4377,13 +4386,13 @@
     </row>
     <row r="133" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E133" s="2" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="F133" s="2" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="H133" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="M133" t="s">
         <v>120</v>
@@ -4394,13 +4403,13 @@
     </row>
     <row r="134" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E134" s="2" t="s">
-        <v>470</v>
+        <v>462</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>470</v>
+        <v>462</v>
       </c>
       <c r="H134" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
       <c r="M134" t="s">
         <v>120</v>
@@ -4411,13 +4420,13 @@
     </row>
     <row r="135" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E135" s="2" t="s">
-        <v>487</v>
+        <v>470</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>487</v>
+        <v>470</v>
       </c>
       <c r="H135" t="s">
-        <v>488</v>
+        <v>471</v>
       </c>
       <c r="M135" t="s">
         <v>120</v>
@@ -4428,13 +4437,13 @@
     </row>
     <row r="136" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E136" s="2" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
       <c r="F136" s="2" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
       <c r="H136" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
       <c r="M136" t="s">
         <v>120</v>
@@ -4445,56 +4454,73 @@
     </row>
     <row r="137" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E137" s="2" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="F137" s="2" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="H137" t="s">
-        <v>499</v>
+        <v>496</v>
+      </c>
+      <c r="M137" t="s">
+        <v>120</v>
+      </c>
+      <c r="N137" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="138" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E138" s="2" t="s">
-        <v>505</v>
+        <v>498</v>
       </c>
       <c r="F138" s="2" t="s">
-        <v>505</v>
+        <v>498</v>
       </c>
       <c r="H138" t="s">
-        <v>511</v>
+        <v>499</v>
       </c>
     </row>
     <row r="139" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E139" s="2" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="F139" s="2" t="s">
-        <v>504</v>
-      </c>
-      <c r="H139" s="2" t="s">
-        <v>506</v>
+        <v>505</v>
+      </c>
+      <c r="H139" t="s">
+        <v>511</v>
       </c>
     </row>
     <row r="140" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E140" s="2" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="F140" s="2" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="H140" s="2" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="141" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E141" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="F141" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="H141" s="2" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="142" spans="5:14" x14ac:dyDescent="0.35">
+      <c r="E142" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="F141" s="2" t="s">
+      <c r="F142" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="H141" t="s">
+      <c r="H142" t="s">
         <v>510</v>
       </c>
     </row>
@@ -4510,8 +4536,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4646,8 +4672,8 @@
         <v>10</v>
       </c>
       <c r="B9" t="str">
-        <f>B10&amp;","&amp;B11&amp;","&amp;B12&amp;","&amp;B13&amp;","&amp;B15&amp;","&amp;B19&amp;",COA"</f>
-        <v>AGR*,COM*,RES*,TRA*,IND*,I??BI*,I??ELC,COK,*ODS*,*OGS*,*OKE*,*OLP*,*OHF*,COA</v>
+        <f>B10&amp;","&amp;B11&amp;","&amp;B12&amp;","&amp;B13&amp;","&amp;B15</f>
+        <v>AGR*,COM*,RES*,TRA*,IND*,I??BI*,I??ELC,COK</v>
       </c>
       <c r="D9" t="s">
         <v>543</v>

</xml_diff>